<commit_message>
correction pour demo fonctionnelle
</commit_message>
<xml_diff>
--- a/Datasets/_Datasets Sent/SR_metadata.xlsx
+++ b/Datasets/_Datasets Sent/SR_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/guillaume_genois_umontreal_ca/Documents/Projet Curation des métadonnées/Datasets/_Datasets Sent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="11_261150FC7C1502149B698B4CD94EF6B8E5158667" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13149C8A-CAD1-4292-B746-6D3ECEA5F7D7}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="11_261150FC7C1502149B698B4CD94EF6B8E5158667" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6E99021-16CF-4A7C-A978-51CD2A9E0A02}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="571" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="571" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestNN" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,32 @@
     <sheet name="DTCPS" sheetId="5" r:id="rId5"/>
     <sheet name="Behave" sheetId="8" r:id="rId6"/>
     <sheet name="TrustSE" sheetId="9" r:id="rId7"/>
-    <sheet name="ModelingAssist" sheetId="12" r:id="rId8"/>
-    <sheet name="ModelGuidance" sheetId="11" r:id="rId9"/>
-    <sheet name="OODP" sheetId="13" r:id="rId10"/>
-    <sheet name="ESPLE" sheetId="14" r:id="rId11"/>
-    <sheet name="SecSelfAdapt" sheetId="15" r:id="rId12"/>
-    <sheet name="SmellReprod" sheetId="16" r:id="rId13"/>
-    <sheet name="ArchiML" sheetId="17" r:id="rId14"/>
-    <sheet name="CodeCompr" sheetId="18" r:id="rId15"/>
-    <sheet name="CodeClone" sheetId="19" r:id="rId16"/>
+    <sheet name="ModelGuidance" sheetId="11" r:id="rId8"/>
+    <sheet name="ESPLE" sheetId="14" r:id="rId9"/>
+    <sheet name="SecSelfAdapt" sheetId="15" r:id="rId10"/>
+    <sheet name="SmellReprod" sheetId="16" r:id="rId11"/>
+    <sheet name="OODP" sheetId="13" r:id="rId12"/>
+    <sheet name="ArchiML" sheetId="17" r:id="rId13"/>
+    <sheet name="CodeCompr" sheetId="18" r:id="rId14"/>
+    <sheet name="CodeClone" sheetId="19" r:id="rId15"/>
+    <sheet name="ModelingAssist" sheetId="12" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="bsec0002" localSheetId="7">ModelingAssist!$E$3</definedName>
+    <definedName name="bsec0002" localSheetId="15">ModelingAssist!$E$3</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -43,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="337">
   <si>
     <t>Link</t>
   </si>
@@ -926,12 +937,360 @@
   <si>
     <t>RQ4. What is the state of the practice on modelling assistance?</t>
   </si>
+  <si>
+    <t>Adaptation is what gives SASs the ability to modify their behavior in response to changes within and outside the system. The type of adaptation possible is usually described in terms of self-* properties.</t>
+  </si>
+  <si>
+    <t>a self-adaptive system consists of two distinct parts, wherein the first part (self-awareness element) interacts with the environment, while the second part cooperates with the first part and deals with any adaptation concerns</t>
+  </si>
+  <si>
+    <t>MAPE-K loop: M stands for Monitoring (system and environment), A for Analysis (what change should happen?), P for Planning (decision(s) to be made), E for Execution (of the action decided), and K for Knowledge base (a shared space that maintains data of the system and its environment).</t>
+  </si>
+  <si>
+    <t>The term adaptation properties refers to the characteristics (non-functional operational properties) of the system that need to be maintained to ascertain the normal operating condition of such a system. Examples of the qualities are: availability, efficiency, performance, reliability, robustness, security, and stability.</t>
+  </si>
+  <si>
+    <t>The Common Attack Pattern Enumeration and Classification (CAPEC)1 scheme postulated by the MITRE Corporation demonstrates a hierarchical framework of different ways by which systems are attacked by a foreign entity. These techniques include Deceptive Interactions, Abuse of Existing Functionality of the System, Data Structure Manipulation, System Resources Manipulation, Injection of Unexpected Items, Employing Probabilistic Techniques, Manipulation of System Timing and State, Collect and Analyze Information, and Circumventing or Subverting Access Control.</t>
+  </si>
+  <si>
+    <t>The CIA triad represents the most commonly used and applied information security model. It is used to provide various organizations and types of systems with knowledge on how to keep data secure. The model consists of the following three aspects: (1) confidentiality — prevention of unauthorized disclosure or use of information assets, (2) integrity — prevention of unauthorized modification of information assets, and (3) availability — ensuring authorized access of information assets when required</t>
+  </si>
+  <si>
+    <t>The term risk represents the joint probabilities of occurrence of various harms and their respective severities.</t>
+  </si>
+  <si>
+    <t>Hazard sources can be classified as internal and external. For example, an internal factor can be mechanical or software related, while external ones can relate to human and environment interaction.</t>
+  </si>
+  <si>
+    <t>(RQ1) Which security attacks and safety hazards in the context of self-adaptive systems are described in the literature?</t>
+  </si>
+  <si>
+    <t>(RQ2) How are security attacks and safety hazards related and which safety mitigation and treatment strategies exist?</t>
+  </si>
+  <si>
+    <t>(RQ3) How are models used in the context of security, safety, and self-adaptive systems, and which analysis approaches are utilized?</t>
+  </si>
+  <si>
+    <t>(RQ4) What open challenges are described in the literature in relation to self-adaptive systems?</t>
+  </si>
+  <si>
+    <t>Peer-reviewed articles</t>
+  </si>
+  <si>
+    <t>Gray and white literature</t>
+  </si>
+  <si>
+    <t>Accessible in full text</t>
+  </si>
+  <si>
+    <t>Non-English articles</t>
+  </si>
+  <si>
+    <t>Published between year 2000 and 2020</t>
+  </si>
+  <si>
+    <t>Secondary studies</t>
+  </si>
+  <si>
+    <t>Discusses explicitly self-adaptation, self-healing or relates to a self-adaptive architecture</t>
+  </si>
+  <si>
+    <t>Addresses security and safety</t>
+  </si>
+  <si>
+    <t>Addresses verification and validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A joint analysis of safety and security aspects in cyber–physical systems (CPS) is necessary, particularly to expose security implications on system safety and vice versa. </t>
+  </si>
+  <si>
+    <t>This study collects and compares security attacks and safety hazards on self-adaptive systems (SAS) described in the literature. In addition, mitigation and treatment strategies, as well as the modeling and analysis approaches, are investigated.</t>
+  </si>
+  <si>
+    <t>This paper aims to investigate the possible reasons for the inconsistencies between studies in the performance of applied machine learning algorithms compared to developers by performing a systematic review. It focuses on the reproducibility of existing studies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code smells are usually understood as patterns in the source code which make it less comprehensible and more error-prone (sometimes they are called antipatterns). </t>
+  </si>
+  <si>
+    <r>
+      <t>reproducibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> means obtaining consistent computational results using the same input data, computational steps, methods, code, and conditions of analysis</t>
+    </r>
+  </si>
+  <si>
+    <t>With the notion of self-management in autonomic computing that allows a computing system to dynamically modify its configuration in response to a change in the system while adhering to business goals, Self-adaptive Systems (SAS) refer to systems that are able to respond to changes in the operating environment thereby affecting the system’s structure, behavior or even the system’s logic.</t>
+  </si>
+  <si>
+    <t>Self-protection describes a group of self-managing systems capable of detecting and mitigating security threats at runtime </t>
+  </si>
+  <si>
+    <t>Self-healing is the ability of a system to return to a functional state after being compromised by an anomalous agent. Self-healing systems endeavor to heal themselves in a similar fashion as a biological system heals from a wound from faults and recovers into normalcy</t>
+  </si>
+  <si>
+    <t>Self-optimization allows for systems to find the optimal solution such as configuration or output</t>
+  </si>
+  <si>
+    <t>Self-configuration is the feature of a system to dynamically and automatically reconfigure itself in response to changes. It allows for the adaptation of a new component or new execution environment within a system with little or no human intervention</t>
+  </si>
+  <si>
+    <r>
+      <t>replicability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> means obtaining consistent results across studies aimed at answering the same scientific question, each of which has obtained its own data</t>
+    </r>
+  </si>
+  <si>
+    <t>RQ1: Is the process of creating code smell machine learning models reproducible in the recent scientific studies on code smell detection using AI/ML methods?</t>
+  </si>
+  <si>
+    <t>RQ2: Is the process of code smell data set acquisition reproducible in the recent scientific studies on code smell detection using AI/ML methods?</t>
+  </si>
+  <si>
+    <t>1. The entry is a single journal paper, chapter of a book or conference proceedings paper which requires peer review (i.e., it is not an editorial, abstract, technical report etc.).</t>
+  </si>
+  <si>
+    <t>2. The paper is written in English.</t>
+  </si>
+  <si>
+    <t>3. The paper was published in 1999 or later.</t>
+  </si>
+  <si>
+    <t>4. Title or abstract of the paper indicates that it is related to software engineering.</t>
+  </si>
+  <si>
+    <t>5. Title or abstract of the paper indicates that at least one code smell/anti-pattern plays an important part of the study.</t>
+  </si>
+  <si>
+    <t>6. Title or abstract of the paper indicates that it might use machine learning techniques.</t>
+  </si>
+  <si>
+    <t>7. Abstract or full text of the paper indicates that it focuses on code smells/anti-patterns in programming languages.</t>
+  </si>
+  <si>
+    <t>8. Abstract or full text of the paper indicates that it focuses on code smells/anti-patterns detection using source code.</t>
+  </si>
+  <si>
+    <t>9. The paper does not focus on techniques for resolving code smells/anti-patterns.</t>
+  </si>
+  <si>
+    <t>10. The paper does not focus on using code smells/anti-patterns as predictors of other code or project traits.</t>
+  </si>
+  <si>
+    <t>11. The paper focuses on detection/prediction of code smells/anti-patterns.</t>
+  </si>
+  <si>
+    <t>12. If the paper is a chapter of a book or conference proceedings publication, its authors have not published a study under the same title in a journal (we want to include the paper once and it may be expected that the journal version includes more details).</t>
+  </si>
+  <si>
+    <t>13. Full text of the paper is available.</t>
+  </si>
+  <si>
+    <t>2. Studies written in English.</t>
+  </si>
+  <si>
+    <t>3. Studies available as full-text.</t>
+  </si>
+  <si>
+    <t>RQ1: What are the most common software architecture design challenges in ML-enabled systems?</t>
+  </si>
+  <si>
+    <t>RQ2: What are the best practices in architecting ML-enabled systems?</t>
+  </si>
+  <si>
+    <t>RQ3: What are the main software architectural design decisions for ML-enabled systems?</t>
+  </si>
+  <si>
+    <t>1. Secondary and tertiary studies (e.g., systematic literature reviews, surveys, etc.).</t>
+  </si>
+  <si>
+    <t>2. Studies in the form of tutorial papers, short papers, poster papers, editorials, and manuals, because they do not provide enough information.</t>
+  </si>
+  <si>
+    <t>The research goal of this work is to identify common challenges, best design practices, and main software architecture design decisions of machine learning enabled systems from the point of view of researchers and practitioners by performing a systematic review.</t>
+  </si>
+  <si>
+    <t>Uncertainty management: properly managing uncertainty permits to avoid significant resource expenses during development. This includes properly (i) architecting data pipelines from training, to deployment, maintenance, and evolution, and (ii) accounting for retraining models and incorporating new data.</t>
+  </si>
+  <si>
+    <t>Quality aspects of ML-enabled systems: properly understanding and managing key quality attributes of ML-enabled systems avoid failures, e.g., boundary erosion, entanglement, hidden feedback loops, undeclared consumers, data dependencies, configuration issues, and changes in the external world</t>
+  </si>
+  <si>
+    <t>Integration with other components: properly designing and integrating ML components with other components, as well as understanding architectural dependencies, is a key aspect for the successful development of effective ML-based systems.</t>
+  </si>
+  <si>
+    <t>This paper proposes a systematic literature review and meta-analysis on code similarity measurement and evaluation techniques to shed light on the existing approaches and their characteristics in different applications.</t>
+  </si>
+  <si>
+    <t>In this paper, we aim to provide a more comprehensive view of the existing knowledge about the impact of different formatting elements on code legibility. We conducted a systematic literature review and identified 15 papers containing human-centric studies that directly compared alternative formatting elements.</t>
+  </si>
+  <si>
+    <t>We use the term understandability to refer to the ease with which developers are able to extract information from a program that is useful for a software development- or maintenance-related task just by reading its source code.</t>
+  </si>
+  <si>
+    <t>code conventions are a body of advice on lexical and syntactic aspects of code, aiming to standardize low-level code design under the assumption that such a systematic approach will make code easier to read, understand, and maintain</t>
+  </si>
+  <si>
+    <t>Comprehension (not reading comprehension, but rather linguistic comprehension) is the process by which given lexical (i.e., word) information, sentences and discourses are interpreted. Decoding and linguistic comprehension are separate components of reading skill.</t>
+  </si>
+  <si>
+    <t>readability: the structural and semantic characteristics of the source code of a program that affect the ability of developers to understand it while reading the code, e.g., programming constructs, coding idioms, and meaningful identifiers</t>
+  </si>
+  <si>
+    <t>legibility: the visual characteristics of the source code of a program, which affect the ability of developers to identify the elements of the code while reading it, such as line breaks, spacing, alignment, indentation, blank lines, identifier capitalization</t>
+  </si>
+  <si>
+    <t>RQ1: What formatting elements at the source code level have been investigated in human-centric studies?</t>
+  </si>
+  <si>
+    <t>RQ2: Which levels of formatting elements have been found to make the source code more legible?</t>
+  </si>
+  <si>
+    <t>Formatting elements, such as spacing, are factors that impact the legibility of the source code and, consequently, may affect the ability of developers to identify the elements of the code while reading it.</t>
+  </si>
+  <si>
+    <t>EC3.: The study is about legibility, readability, or understandability metrics.</t>
+  </si>
+  <si>
+    <t>EC1.: The study is clearly irrelevant to our research questions, i.e., it is not primarily related to source code comprehension, readability, legibility, or hard-to-understand code, or does not involve any comparison of different ways of writing code.</t>
+  </si>
+  <si>
+    <t>EC2.: The study is not a full paper (e.g., PhD theses or 4-page papers), is not written in English, or was not peer-reviewed.</t>
+  </si>
+  <si>
+    <t>EC4.: The study is about program comprehension aids, such as visualizations or other forms of analysis or sensory aids, e.g., trace-based execution, code summarization, and character encodings supporting colors.</t>
+  </si>
+  <si>
+    <t>EC5.: The study focuses on accessibility, e.g., targets individuals with visual impairments or neurodiverse developers.</t>
+  </si>
+  <si>
+    <t>IC1 (Scope).: The study must be primarily related to legibility.</t>
+  </si>
+  <si>
+    <t>IC2 (Methodology).: The study must be or contain a controlled experiment, quasi-experiment, or survey involving human subjects.</t>
+  </si>
+  <si>
+    <t>IC3 (Comparison).: The study must directly compare alternative formatting elements in terms of code legibility, and the alternatives must be clearly identifiable.</t>
+  </si>
+  <si>
+    <t>IC4 (Granularity).: The study must target fine-grained program elements and low-level/limited-scope programming activities. Not design or comments, but implementation.</t>
+  </si>
+  <si>
+    <t>Architecting ML-enabled systems: ????</t>
+  </si>
+  <si>
+    <t>RQ1: What are the existing code similarity measurement approaches and techniques, and what are their advantages and disadvantages?</t>
+  </si>
+  <si>
+    <t>RQ2: What are the applications of code similarity measurement in software engineering activities and tasks?</t>
+  </si>
+  <si>
+    <t>RQ3: What are the existing code similarity measurement tools, and which programming languages are supported by each tool?</t>
+  </si>
+  <si>
+    <t>RQ4: Which software projects and datasets have been used to build and evaluate code similarity measurement tools?</t>
+  </si>
+  <si>
+    <t>RQ5: How is the performance of the existing code similarity measurement methods?</t>
+  </si>
+  <si>
+    <t>RQ6: What are the existing challenges and opportunities in source code similarity measurement?</t>
+  </si>
+  <si>
+    <t>EC4: Articles that did not directly discuss a source code similarity measurement approach in their abstract were removed. For example, some papers have discussed binary code similarity.</t>
+  </si>
+  <si>
+    <t>EC6: Theses, books, journal covers and metadata, secondary, tertiary, empirical, and case studies were removed.</t>
+  </si>
+  <si>
+    <t>EC1: The articles repeated in citation databases were removed. We kept only one version of each duplicated article.</t>
+  </si>
+  <si>
+    <t>EC2: Articles whose main text was written in any language other than English or only their abstract and keywords were in English were eliminated.</t>
+  </si>
+  <si>
+    <t>EC3: Articles whose total text was less than three pages were removed. After reviewing them, we removed these articles and ensured they did not contain significant contributions. If there are good clues in these articles to find other suitable topics and articles, we consider these clues while applying the inclusion criteria and snowballing phases.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EC5: The papers that had not proposed an </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>automated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> approach for source code similarity measurement were removed. We excluded these articles since the similarity measurement technique was necessary when classifying methods.</t>
+    </r>
+  </si>
+  <si>
+    <t>IC1: At least one keyword of the article existed in our search string.</t>
+  </si>
+  <si>
+    <t>IC2: The title or abstract of the article is about the measurement or application of the source code similarity.</t>
+  </si>
+  <si>
+    <t>IC3: The article has been cited at least once. This criterion was considered only for articles that were published before 2021. Using this condition, we could ensure other researchers in the community have considered the paper.</t>
+  </si>
+  <si>
+    <t>IC4: The conference paper is considered if it does not have any journal extension. Otherwise, only its journal extension was included since articles published in a journal often offer more complete descriptions than their conferences counterpart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source code similarity is a concept used to measure the similarity degree between a piece of code snippets with respect to the text, syntax, and semantics. Although there is no well-established definition for code similarity in general, typically, the similarity score for any two code snippets , is measured with a real number where the higher the score is, the more similar and are. </t>
+  </si>
+  <si>
+    <t>Two code snippets c1, c2 are clones if they are similar according to some definition of similarity.</t>
+  </si>
+  <si>
+    <t>Cross-language clones typically occur when a codebase is prepared to use in different environments for portability. For instance, the main codebase of the game is actually the same while building a game for different operating systems, and there are slight differences for each operating system.</t>
+  </si>
+  <si>
+    <t>1. Studies subject to peer review.</t>
+  </si>
+  <si>
+    <t>5. Studies describing software architecture best practices for machine learning systems.</t>
+  </si>
+  <si>
+    <t>4. Studies discussing software architecture challenges for machine learning systems.</t>
+  </si>
+  <si>
+    <t>6. Studies describing software architecture design decisions for machine learning systems.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -959,6 +1318,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -981,7 +1362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1016,17 +1397,243 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="77">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1155,78 +1762,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1377,105 +1912,105 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FDFBD496-016F-4ECA-9794-10AC24C99732}" name="Tableau2911" displayName="Tableau2911" ref="A1:F18" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{5A2F9E98-03A4-498A-82BF-D2D73CA51CB7}" name="Tableau213" displayName="Tableau213" ref="A1:F14" totalsRowShown="0" dataDxfId="28">
+  <autoFilter ref="A1:F14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FDCB47A1-0B7A-4D02-BBB1-DC2A15B6A56D}" name="Link" dataDxfId="22" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="2" xr3:uid="{DDE08B9B-69C0-4189-B0DA-E7EC9F30CCEE}" name="Topic" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{186DAECF-7340-44D1-8A78-F8D7145947C5}" name="Definitions" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{FAC2FCB2-F895-4CDC-8328-7CFD3426D2DF}" name="Research questions" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{908D7060-F82C-4332-8F23-26E64DDAA302}" name="Inclusion criteria" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{5EE73402-BB91-4051-B287-7937FF24FD8F}" name="Exclusion criteria" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{E6D737CD-B321-46DA-8374-652105AF0383}" name="Link" dataDxfId="27" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{68496D58-37AD-45B9-A593-20F0C9B014D1}" name="Topic" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{C09773DB-C6C2-4767-BD01-79FAD216D591}" name="Definitions" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{E4A2A5C1-6CE6-4210-B508-AAE650E5BA19}" name="Research questions" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{B2E60AD9-79CC-4369-B5EE-343E7B546368}" name="Inclusion criteria" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{2DF14E44-563C-4AB5-947D-C94D914767B7}" name="Exclusion criteria" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9F21A95C-CE81-4F39-8382-77F8CA6AFF63}" name="Tableau291112" displayName="Tableau291112" ref="A1:F7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:F7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7DB03802-95DA-4681-BB2D-697C4398F5F0}" name="Tableau21314" displayName="Tableau21314" ref="A1:F27" totalsRowShown="0" dataDxfId="21">
+  <autoFilter ref="A1:F27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{838F3C3C-D92E-43FC-91B8-4261F04C324A}" name="Link" dataDxfId="14" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="2" xr3:uid="{63BD9556-D4C6-468F-9B25-09DC5C288A3F}" name="Topic" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{60972BAA-0127-4CD0-9709-B240266E1667}" name="Definitions" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{413B6281-F4E9-4593-8527-02D2109423F4}" name="Research questions" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{4C973CE1-25AD-4019-B8BB-C487D96F6512}" name="Inclusion criteria" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{EB2C5248-8FB4-4A74-AE93-379C9129E38C}" name="Exclusion criteria" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{FC343DB5-06F4-425D-9DC0-5B41FFA2FBE6}" name="Link" dataDxfId="20" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{CDB83B9E-0E92-4773-BB5D-39BB8B315782}" name="Topic" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F9C6F6BD-052A-4EF8-A3CD-93FC88EDAB38}" name="Definitions" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{BF2A8F62-537D-449E-9268-52D99DEE5EB1}" name="Research questions" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{171D2F36-56C8-497A-9EEA-89559EAA54DE}" name="Inclusion criteria" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{9D709ACA-BBAE-4B49-BAB0-FD61DBE8DBD2}" name="Exclusion criteria" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{5A2F9E98-03A4-498A-82BF-D2D73CA51CB7}" name="Tableau213" displayName="Tableau213" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FDFBD496-016F-4ECA-9794-10AC24C99732}" name="Tableau2911" displayName="Tableau2911" ref="A1:F18" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E6D737CD-B321-46DA-8374-652105AF0383}" name="Link" dataDxfId="0" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="2" xr3:uid="{68496D58-37AD-45B9-A593-20F0C9B014D1}" name="Topic"/>
-    <tableColumn id="3" xr3:uid="{C09773DB-C6C2-4767-BD01-79FAD216D591}" name="Definitions"/>
-    <tableColumn id="4" xr3:uid="{E4A2A5C1-6CE6-4210-B508-AAE650E5BA19}" name="Research questions"/>
-    <tableColumn id="5" xr3:uid="{B2E60AD9-79CC-4369-B5EE-343E7B546368}" name="Inclusion criteria"/>
-    <tableColumn id="6" xr3:uid="{2DF14E44-563C-4AB5-947D-C94D914767B7}" name="Exclusion criteria"/>
+    <tableColumn id="1" xr3:uid="{FDCB47A1-0B7A-4D02-BBB1-DC2A15B6A56D}" name="Link" dataDxfId="42" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{DDE08B9B-69C0-4189-B0DA-E7EC9F30CCEE}" name="Topic" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{186DAECF-7340-44D1-8A78-F8D7145947C5}" name="Definitions" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{FAC2FCB2-F895-4CDC-8328-7CFD3426D2DF}" name="Research questions" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{908D7060-F82C-4332-8F23-26E64DDAA302}" name="Inclusion criteria" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{5EE73402-BB91-4051-B287-7937FF24FD8F}" name="Exclusion criteria" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7DB03802-95DA-4681-BB2D-697C4398F5F0}" name="Tableau21314" displayName="Tableau21314" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{31C206B0-0636-4AE1-BC85-DE37B5017FE8}" name="Tableau2131415" displayName="Tableau2131415" ref="A1:F9" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FC343DB5-06F4-425D-9DC0-5B41FFA2FBE6}" name="Link"/>
-    <tableColumn id="2" xr3:uid="{CDB83B9E-0E92-4773-BB5D-39BB8B315782}" name="Topic"/>
-    <tableColumn id="3" xr3:uid="{F9C6F6BD-052A-4EF8-A3CD-93FC88EDAB38}" name="Definitions"/>
-    <tableColumn id="4" xr3:uid="{BF2A8F62-537D-449E-9268-52D99DEE5EB1}" name="Research questions"/>
-    <tableColumn id="5" xr3:uid="{171D2F36-56C8-497A-9EEA-89559EAA54DE}" name="Inclusion criteria"/>
-    <tableColumn id="6" xr3:uid="{9D709ACA-BBAE-4B49-BAB0-FD61DBE8DBD2}" name="Exclusion criteria"/>
+    <tableColumn id="1" xr3:uid="{D87B9C92-6374-4C10-A084-10CC492629FC}" name="Link" dataDxfId="13" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{CD2F3414-C6D7-4E61-9E72-93C97BCDD114}" name="Topic" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{D80F43C9-BB22-4522-88E7-91959651AADD}" name="Definitions" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{0288A10D-212D-42FD-A867-A51DAA672684}" name="Research questions" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{4D82ABCE-299D-4029-8C52-7059AA8D3197}" name="Inclusion criteria" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{79823B39-89D0-4F7D-8910-7CE320F0C02C}" name="Exclusion criteria" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{31C206B0-0636-4AE1-BC85-DE37B5017FE8}" name="Tableau2131415" displayName="Tableau2131415" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{624D388E-2A5C-40C9-9E6F-E3E63300AF20}" name="Tableau213141516" displayName="Tableau213141516" ref="A1:F11" totalsRowShown="0">
+  <autoFilter ref="A1:F11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D87B9C92-6374-4C10-A084-10CC492629FC}" name="Link"/>
-    <tableColumn id="2" xr3:uid="{CD2F3414-C6D7-4E61-9E72-93C97BCDD114}" name="Topic"/>
-    <tableColumn id="3" xr3:uid="{D80F43C9-BB22-4522-88E7-91959651AADD}" name="Definitions"/>
-    <tableColumn id="4" xr3:uid="{0288A10D-212D-42FD-A867-A51DAA672684}" name="Research questions"/>
-    <tableColumn id="5" xr3:uid="{4D82ABCE-299D-4029-8C52-7059AA8D3197}" name="Inclusion criteria"/>
-    <tableColumn id="6" xr3:uid="{79823B39-89D0-4F7D-8910-7CE320F0C02C}" name="Exclusion criteria"/>
+    <tableColumn id="1" xr3:uid="{0E89DED2-A413-40D7-AFCE-ABDBA5E8D895}" name="Link" dataDxfId="7" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{05BD4CAF-CDAC-44D2-897A-8BEE5237E203}" name="Topic" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C353998E-E140-4127-B64E-8EFB167C6065}" name="Definitions" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{EE9EA9B2-4685-4E73-8C01-D1077262DBAA}" name="Research questions"/>
+    <tableColumn id="5" xr3:uid="{55541BC9-185D-4331-85A5-7984156AA235}" name="Inclusion criteria" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{578A67C7-B5B9-47E0-8CDC-8CA8B9815B61}" name="Exclusion criteria" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{624D388E-2A5C-40C9-9E6F-E3E63300AF20}" name="Tableau213141516" displayName="Tableau213141516" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{8913C4D0-9F39-448A-A1E3-4EFE35F40EBC}" name="Tableau21314151617" displayName="Tableau21314151617" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0E89DED2-A413-40D7-AFCE-ABDBA5E8D895}" name="Link"/>
-    <tableColumn id="2" xr3:uid="{05BD4CAF-CDAC-44D2-897A-8BEE5237E203}" name="Topic"/>
-    <tableColumn id="3" xr3:uid="{C353998E-E140-4127-B64E-8EFB167C6065}" name="Definitions"/>
-    <tableColumn id="4" xr3:uid="{EE9EA9B2-4685-4E73-8C01-D1077262DBAA}" name="Research questions"/>
-    <tableColumn id="5" xr3:uid="{55541BC9-185D-4331-85A5-7984156AA235}" name="Inclusion criteria"/>
-    <tableColumn id="6" xr3:uid="{578A67C7-B5B9-47E0-8CDC-8CA8B9815B61}" name="Exclusion criteria"/>
+    <tableColumn id="1" xr3:uid="{7899E231-E1EF-4D74-BF25-12348DCCD5F8}" name="Link" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{77D42AEE-2E64-4685-A71B-AF2A47199AD9}" name="Topic" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E561F99E-339F-420E-BBCC-D5D0AFF36212}" name="Definitions"/>
+    <tableColumn id="4" xr3:uid="{78D9E0D1-6032-4217-AC34-7285A376FD45}" name="Research questions"/>
+    <tableColumn id="5" xr3:uid="{801A0AB8-BB70-4E10-98B1-991DABBACE42}" name="Inclusion criteria" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{861623C1-C580-4E86-B140-D9708534C453}" name="Exclusion criteria" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{8913C4D0-9F39-448A-A1E3-4EFE35F40EBC}" name="Tableau21314151617" displayName="Tableau21314151617" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{278F8B2F-F0C8-459C-B732-E0DF0BBF5987}" name="Tableau210" displayName="Tableau210" ref="A1:F6" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:F6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7899E231-E1EF-4D74-BF25-12348DCCD5F8}" name="Link"/>
-    <tableColumn id="2" xr3:uid="{77D42AEE-2E64-4685-A71B-AF2A47199AD9}" name="Topic"/>
-    <tableColumn id="3" xr3:uid="{E561F99E-339F-420E-BBCC-D5D0AFF36212}" name="Definitions"/>
-    <tableColumn id="4" xr3:uid="{78D9E0D1-6032-4217-AC34-7285A376FD45}" name="Research questions"/>
-    <tableColumn id="5" xr3:uid="{801A0AB8-BB70-4E10-98B1-991DABBACE42}" name="Inclusion criteria"/>
-    <tableColumn id="6" xr3:uid="{861623C1-C580-4E86-B140-D9708534C453}" name="Exclusion criteria"/>
+    <tableColumn id="1" xr3:uid="{429546C4-0EF0-4CF1-8BA6-49B4FEA593CC}" name="Link" dataDxfId="58" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{1068B8E7-2BA3-4E76-AD4F-3235E94A81FD}" name="Topic" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{6FD76E99-95FA-4A87-8A5A-4C251967636E}" name="Definitions" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{E523BF9C-7A65-41F3-9A06-38FF62A88F17}" name="Research questions" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{89ACB3EB-94D0-4CC3-A8EC-0F565935580D}" name="Inclusion criteria" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{297CE02D-609D-422B-9B38-47728FD82851}" name="Exclusion criteria" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1542,60 +2077,60 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{32AEF01A-D6D4-4E34-B5FC-2BDF6AA2DCB9}" name="Tableau27" displayName="Tableau27" ref="A1:F15" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{32AEF01A-D6D4-4E34-B5FC-2BDF6AA2DCB9}" name="Tableau27" displayName="Tableau27" ref="A1:F15" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="A1:F15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5EE6EC3B-1DDD-42C3-904C-1948CD51AFA8}" name="Link" dataDxfId="46" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="2" xr3:uid="{DBE62ADB-0C08-48DF-840D-B5F68F0BD294}" name="Topic" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{5AB0A917-8CEF-491B-B521-7DEC7EBFE048}" name="Definitions" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{F0EE042E-60EC-4201-895C-8561121228E4}" name="Research questions" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{3FAAC23B-2184-4130-A3E9-0E54D8CC697A}" name="Inclusion criteria" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{8497CC3A-517D-40E4-8145-069777E87198}" name="Exclusion criteria" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{5EE6EC3B-1DDD-42C3-904C-1948CD51AFA8}" name="Link" dataDxfId="74" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{DBE62ADB-0C08-48DF-840D-B5F68F0BD294}" name="Topic" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{5AB0A917-8CEF-491B-B521-7DEC7EBFE048}" name="Definitions" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{F0EE042E-60EC-4201-895C-8561121228E4}" name="Research questions" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{3FAAC23B-2184-4130-A3E9-0E54D8CC697A}" name="Inclusion criteria" dataDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{8497CC3A-517D-40E4-8145-069777E87198}" name="Exclusion criteria" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FFFC1710-CEC4-4940-8764-F55BA276EFF8}" name="Tableau278" displayName="Tableau278" ref="A1:F16" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FFFC1710-CEC4-4940-8764-F55BA276EFF8}" name="Tableau278" displayName="Tableau278" ref="A1:F16" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:F16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F3834B42-F426-43A1-A266-6B45913B3320}" name="Link" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{0303F2C9-CEBE-4B6F-BB4C-9B55ABCA436B}" name="Topic" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{C06B9FAB-27A1-48E3-91D5-456E066CD71A}" name="Definitions" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{31F1E629-A4C3-4ECE-83F4-88FD122A214F}" name="Research questions" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{152171F9-FD5F-4A47-9155-D0D843C9B045}" name="Inclusion criteria" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{4886FC61-7E8D-4E88-B42E-D57FAE612318}" name="Exclusion criteria" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{F3834B42-F426-43A1-A266-6B45913B3320}" name="Link" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{0303F2C9-CEBE-4B6F-BB4C-9B55ABCA436B}" name="Topic" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{C06B9FAB-27A1-48E3-91D5-456E066CD71A}" name="Definitions" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{31F1E629-A4C3-4ECE-83F4-88FD122A214F}" name="Research questions" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{152171F9-FD5F-4A47-9155-D0D843C9B045}" name="Inclusion criteria" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{4886FC61-7E8D-4E88-B42E-D57FAE612318}" name="Exclusion criteria" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{278F8B2F-F0C8-459C-B732-E0DF0BBF5987}" name="Tableau210" displayName="Tableau210" ref="A1:F6" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:F6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A5982F48-6CDA-4074-B33A-AA9859EE1DA1}" name="Tableau29" displayName="Tableau29" ref="A1:F34" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+  <autoFilter ref="A1:F34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{429546C4-0EF0-4CF1-8BA6-49B4FEA593CC}" name="Link" dataDxfId="8" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="2" xr3:uid="{1068B8E7-2BA3-4E76-AD4F-3235E94A81FD}" name="Topic" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{6FD76E99-95FA-4A87-8A5A-4C251967636E}" name="Definitions" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{E523BF9C-7A65-41F3-9A06-38FF62A88F17}" name="Research questions" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{89ACB3EB-94D0-4CC3-A8EC-0F565935580D}" name="Inclusion criteria" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{297CE02D-609D-422B-9B38-47728FD82851}" name="Exclusion criteria" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{D7D90E9B-30D8-419E-A8C3-FEBE28A75DE8}" name="Link" dataDxfId="50" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{CA0C295F-0AE1-408A-AB75-8010A4BD1153}" name="Topic" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{EEC776FF-8C7C-42E3-96D6-CAA1243CD0B4}" name="Definitions" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{9100B27D-3AA5-48A3-8CAA-F0D85852F2F6}" name="Research questions" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{CEF82D53-E350-4632-A007-C8D8D040A237}" name="Inclusion criteria" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{48859DA7-2ABA-4F18-8BD5-4FD5EC454262}" name="Exclusion criteria" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A5982F48-6CDA-4074-B33A-AA9859EE1DA1}" name="Tableau29" displayName="Tableau29" ref="A1:F34" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="A1:F34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9F21A95C-CE81-4F39-8382-77F8CA6AFF63}" name="Tableau291112" displayName="Tableau291112" ref="A1:F7" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:F7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D7D90E9B-30D8-419E-A8C3-FEBE28A75DE8}" name="Link" dataDxfId="30" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="2" xr3:uid="{CA0C295F-0AE1-408A-AB75-8010A4BD1153}" name="Topic" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{EEC776FF-8C7C-42E3-96D6-CAA1243CD0B4}" name="Definitions" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{9100B27D-3AA5-48A3-8CAA-F0D85852F2F6}" name="Research questions" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{CEF82D53-E350-4632-A007-C8D8D040A237}" name="Inclusion criteria" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{48859DA7-2ABA-4F18-8BD5-4FD5EC454262}" name="Exclusion criteria" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{838F3C3C-D92E-43FC-91B8-4261F04C324A}" name="Link" dataDxfId="34" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" xr3:uid="{63BD9556-D4C6-468F-9B25-09DC5C288A3F}" name="Topic" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{60972BAA-0127-4CD0-9709-B240266E1667}" name="Definitions" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{413B6281-F4E9-4593-8527-02D2109423F4}" name="Research questions" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{4C973CE1-25AD-4019-B8BB-C487D96F6512}" name="Inclusion criteria" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{EB2C5248-8FB4-4A74-AE93-379C9129E38C}" name="Exclusion criteria" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1896,6 +2431,514 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBBFA14-1322-4E98-87BF-3DDDDE43EA58}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CFA06BC9-342A-4258-BB2D-EEF37B0A8C08}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A8C2DB-A48E-4FCA-BDC2-A672730951E2}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="174" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="6"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="6"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="6"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="6"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{457CBEE1-CF33-47AE-8976-CFD6F1F07DD7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BE27D1-FC8B-4FCC-9577-8A1390EFCE79}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -2098,124 +3141,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508C21AA-42CD-4436-89CB-908061F0F07E}">
-  <dimension ref="A1:F7"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A605BA-CD4A-4954-943D-B03D1FA3E84E}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="24.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.6328125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="232" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="D3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="D4" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="F5" s="10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="F6" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="F7" s="10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4DB96C03-3D06-471F-987B-CD4A37D61BC4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBBFA14-1322-4E98-87BF-3DDDDE43EA58}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2247,14 +3178,257 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>224</v>
-      </c>
+    <row r="2" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" ht="116" x14ac:dyDescent="0.35">
+      <c r="A5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="18"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CFA06BC9-342A-4258-BB2D-EEF37B0A8C08}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4083498-8577-408D-A18A-855DB0003E6D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C5532A-FC34-407C-96B5-FEC1C4716903}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="23.36328125" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="203" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="F11" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BA3D02C7-7F6F-4396-B722-992C8EC4FBA5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2264,12 +3438,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A8C2DB-A48E-4FCA-BDC2-A672730951E2}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F83910-2967-4B85-A916-FCE29DD58188}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2278,7 +3452,7 @@
     <col min="3" max="3" width="37.7265625" customWidth="1"/>
     <col min="4" max="4" width="40.453125" customWidth="1"/>
     <col min="5" max="5" width="28.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -2297,27 +3471,148 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>223</v>
-      </c>
+    <row r="2" spans="1:6" ht="145" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="174" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="1"/>
+      <c r="D6" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="12"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="1"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="1"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="1"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="1"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
+      <c r="B12" s="1"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="12"/>
+      <c r="B13" s="1"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{47CA9A73-8496-4A88-B275-9B18DCF6C1D7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A605BA-CD4A-4954-943D-B03D1FA3E84E}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B6DEE2-F317-44E3-8C00-B83AE33B56C8}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2325,145 +3620,104 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="1" max="2" width="24.1796875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="10.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>222</v>
+    <row r="2" spans="1:6" ht="290" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11"/>
+      <c r="D4" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="D5" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="F6" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2FE4ABE4-FD59-436D-BE9B-43A41F323EE4}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4C01A702-A952-4255-8374-A3AFAA1213A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C5532A-FC34-407C-96B5-FEC1C4716903}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F83910-2967-4B85-A916-FCE29DD58188}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3272,118 +4526,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B6DEE2-F317-44E3-8C00-B83AE33B56C8}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="24.1796875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="10.6328125" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="290" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="D4" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="11"/>
-      <c r="D5" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="F6" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2FE4ABE4-FD59-436D-BE9B-43A41F323EE4}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{4C01A702-A952-4255-8374-A3AFAA1213A1}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13ACB25F-A7EC-4321-8707-32021CCE86B3}">
   <dimension ref="A1:F34"/>
   <sheetViews>
@@ -3582,4 +4724,116 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508C21AA-42CD-4436-89CB-908061F0F07E}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="24.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.6328125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="232" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="D3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="D4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="F5" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="F6" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="F7" s="10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4DB96C03-3D06-471F-987B-CD4A37D61BC4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>